<commit_message>
working on regex for dates
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\Programming Skills Enhancement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C59A002-1D66-43C0-A582-B2F6E6354E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813D7083-CCCB-45EB-ADD4-8648C8336471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D3C0452C-0C03-4F21-9527-4AC5B9535FA6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3C0452C-0C03-4F21-9527-4AC5B9535FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
move validation to a different file
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\Programming Skills Enhancement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanju\Documents\Github_Workstation\Programming_Skills_Enhancement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2E7513-1DA8-4FB8-848D-E437673090F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC8C18-43CA-48B1-BC79-B75668AD8D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D3C0452C-0C03-4F21-9527-4AC5B9535FA6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{D3C0452C-0C03-4F21-9527-4AC5B9535FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Title3</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>11/10/20a20</t>
+  </si>
+  <si>
+    <t>12/18/20a20</t>
   </si>
 </sst>
 </file>
@@ -463,27 +466,27 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.53125" customWidth="1"/>
+    <col min="5" max="5" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1">
-        <v>37608</v>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -502,7 +505,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -510,7 +513,7 @@
         <v>44146</v>
       </c>
       <c r="C2" s="1">
-        <v>37609</v>
+        <v>44184</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -528,7 +531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -536,7 +539,7 @@
         <v>44147</v>
       </c>
       <c r="C3" s="1">
-        <v>37610</v>
+        <v>44185</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -554,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>4</v>
       </c>
@@ -562,7 +565,7 @@
         <v>44148</v>
       </c>
       <c r="C4" s="1">
-        <v>37611</v>
+        <v>44186</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -580,7 +583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -588,7 +591,7 @@
         <v>44149</v>
       </c>
       <c r="C5" s="1">
-        <v>37612</v>
+        <v>44187</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -606,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>6</v>
       </c>
@@ -614,7 +617,7 @@
         <v>44150</v>
       </c>
       <c r="C6" s="1">
-        <v>37613</v>
+        <v>44188</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -632,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>7</v>
       </c>
@@ -640,7 +643,7 @@
         <v>44151</v>
       </c>
       <c r="C7" s="1">
-        <v>37614</v>
+        <v>44189</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -658,7 +661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>8</v>
       </c>
@@ -666,7 +669,7 @@
         <v>44152</v>
       </c>
       <c r="C8" s="1">
-        <v>37615</v>
+        <v>44190</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -684,7 +687,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9</v>
       </c>
@@ -692,7 +695,7 @@
         <v>44153</v>
       </c>
       <c r="C9" s="1">
-        <v>37616</v>
+        <v>44191</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -710,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>10</v>
       </c>
@@ -718,7 +721,7 @@
         <v>44154</v>
       </c>
       <c r="C10" s="1">
-        <v>37617</v>
+        <v>44192</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
working on import of data into sqllite
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanju\Documents\Github_Workstation\Programming_Skills_Enhancement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC8C18-43CA-48B1-BC79-B75668AD8D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4584D8-B799-4038-9C6B-DCD16D5EA61C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{D3C0452C-0C03-4F21-9527-4AC5B9535FA6}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -525,7 +525,7 @@
         <v>17</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>

</xml_diff>